<commit_message>
Added to Gantt Chart
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KamaldeepSingh/Documents/University/Software Projects/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14445" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pre Gantt Chart" sheetId="1" r:id="rId1"/>
     <sheet name="After Gantt Chart" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Group I</t>
   </si>
@@ -80,12 +75,15 @@
   <si>
     <t>April</t>
   </si>
+  <si>
+    <t>GitHub Setup</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -115,7 +113,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,6 +123,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -209,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -227,6 +237,16 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -242,16 +262,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -309,7 +321,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -344,7 +356,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -521,216 +533,216 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:HF17"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="A5" zoomScaleNormal="93" zoomScalePageLayoutView="93" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:214" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:214" ht="15.95" customHeight="1">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="M1" s="10" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="M1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
-      <c r="AH1" s="10"/>
-      <c r="AI1" s="10"/>
-      <c r="AJ1" s="10"/>
-      <c r="AK1" s="10"/>
-      <c r="AL1" s="10"/>
-      <c r="AM1" s="10"/>
-      <c r="AN1" s="10"/>
-      <c r="AO1" s="10"/>
-      <c r="AP1" s="10"/>
-      <c r="AQ1" s="10"/>
-      <c r="AR1" s="10"/>
-      <c r="AS1" s="10"/>
-      <c r="AT1" s="10"/>
-      <c r="AU1" s="10"/>
-    </row>
-    <row r="2" spans="1:214" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="10"/>
-      <c r="AB2" s="10"/>
-      <c r="AC2" s="10"/>
-      <c r="AD2" s="10"/>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="10"/>
-      <c r="AG2" s="10"/>
-      <c r="AH2" s="10"/>
-      <c r="AI2" s="10"/>
-      <c r="AJ2" s="10"/>
-      <c r="AK2" s="10"/>
-      <c r="AL2" s="10"/>
-      <c r="AM2" s="10"/>
-      <c r="AN2" s="10"/>
-      <c r="AO2" s="10"/>
-      <c r="AP2" s="10"/>
-      <c r="AQ2" s="10"/>
-      <c r="AR2" s="10"/>
-      <c r="AS2" s="10"/>
-      <c r="AT2" s="10"/>
-      <c r="AU2" s="10"/>
-    </row>
-    <row r="3" spans="1:214" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="10"/>
-      <c r="AB3" s="10"/>
-      <c r="AC3" s="10"/>
-      <c r="AD3" s="10"/>
-      <c r="AE3" s="10"/>
-      <c r="AF3" s="10"/>
-      <c r="AG3" s="10"/>
-      <c r="AH3" s="10"/>
-      <c r="AI3" s="10"/>
-      <c r="AJ3" s="10"/>
-      <c r="AK3" s="10"/>
-      <c r="AL3" s="10"/>
-      <c r="AM3" s="10"/>
-      <c r="AN3" s="10"/>
-      <c r="AO3" s="10"/>
-      <c r="AP3" s="10"/>
-      <c r="AQ3" s="10"/>
-      <c r="AR3" s="10"/>
-      <c r="AS3" s="10"/>
-      <c r="AT3" s="10"/>
-      <c r="AU3" s="10"/>
-    </row>
-    <row r="4" spans="1:214" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
-      <c r="AA4" s="10"/>
-      <c r="AB4" s="10"/>
-      <c r="AC4" s="10"/>
-      <c r="AD4" s="10"/>
-      <c r="AE4" s="10"/>
-      <c r="AF4" s="10"/>
-      <c r="AG4" s="10"/>
-      <c r="AH4" s="10"/>
-      <c r="AI4" s="10"/>
-      <c r="AJ4" s="10"/>
-      <c r="AK4" s="10"/>
-      <c r="AL4" s="10"/>
-      <c r="AM4" s="10"/>
-      <c r="AN4" s="10"/>
-      <c r="AO4" s="10"/>
-      <c r="AP4" s="10"/>
-      <c r="AQ4" s="10"/>
-      <c r="AR4" s="10"/>
-      <c r="AS4" s="10"/>
-      <c r="AT4" s="10"/>
-      <c r="AU4" s="10"/>
-    </row>
-    <row r="5" spans="1:214" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:214" s="3" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="14"/>
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="14"/>
+      <c r="AI1" s="14"/>
+      <c r="AJ1" s="14"/>
+      <c r="AK1" s="14"/>
+      <c r="AL1" s="14"/>
+      <c r="AM1" s="14"/>
+      <c r="AN1" s="14"/>
+      <c r="AO1" s="14"/>
+      <c r="AP1" s="14"/>
+      <c r="AQ1" s="14"/>
+      <c r="AR1" s="14"/>
+      <c r="AS1" s="14"/>
+      <c r="AT1" s="14"/>
+      <c r="AU1" s="14"/>
+    </row>
+    <row r="2" spans="1:214" ht="15.95" customHeight="1">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="14"/>
+      <c r="AE2" s="14"/>
+      <c r="AF2" s="14"/>
+      <c r="AG2" s="14"/>
+      <c r="AH2" s="14"/>
+      <c r="AI2" s="14"/>
+      <c r="AJ2" s="14"/>
+      <c r="AK2" s="14"/>
+      <c r="AL2" s="14"/>
+      <c r="AM2" s="14"/>
+      <c r="AN2" s="14"/>
+      <c r="AO2" s="14"/>
+      <c r="AP2" s="14"/>
+      <c r="AQ2" s="14"/>
+      <c r="AR2" s="14"/>
+      <c r="AS2" s="14"/>
+      <c r="AT2" s="14"/>
+      <c r="AU2" s="14"/>
+    </row>
+    <row r="3" spans="1:214" ht="15.95" customHeight="1">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14"/>
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="14"/>
+      <c r="AC3" s="14"/>
+      <c r="AD3" s="14"/>
+      <c r="AE3" s="14"/>
+      <c r="AF3" s="14"/>
+      <c r="AG3" s="14"/>
+      <c r="AH3" s="14"/>
+      <c r="AI3" s="14"/>
+      <c r="AJ3" s="14"/>
+      <c r="AK3" s="14"/>
+      <c r="AL3" s="14"/>
+      <c r="AM3" s="14"/>
+      <c r="AN3" s="14"/>
+      <c r="AO3" s="14"/>
+      <c r="AP3" s="14"/>
+      <c r="AQ3" s="14"/>
+      <c r="AR3" s="14"/>
+      <c r="AS3" s="14"/>
+      <c r="AT3" s="14"/>
+      <c r="AU3" s="14"/>
+    </row>
+    <row r="4" spans="1:214" ht="15.95" customHeight="1">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="14"/>
+      <c r="AB4" s="14"/>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="14"/>
+      <c r="AE4" s="14"/>
+      <c r="AF4" s="14"/>
+      <c r="AG4" s="14"/>
+      <c r="AH4" s="14"/>
+      <c r="AI4" s="14"/>
+      <c r="AJ4" s="14"/>
+      <c r="AK4" s="14"/>
+      <c r="AL4" s="14"/>
+      <c r="AM4" s="14"/>
+      <c r="AN4" s="14"/>
+      <c r="AO4" s="14"/>
+      <c r="AP4" s="14"/>
+      <c r="AQ4" s="14"/>
+      <c r="AR4" s="14"/>
+      <c r="AS4" s="14"/>
+      <c r="AT4" s="14"/>
+      <c r="AU4" s="14"/>
+    </row>
+    <row r="5" spans="1:214" ht="18" customHeight="1"/>
+    <row r="6" spans="1:214" s="3" customFormat="1" ht="63" customHeight="1">
       <c r="C6" s="1">
         <v>42284</v>
       </c>
@@ -1320,7 +1332,7 @@
       <c r="HE6" s="1"/>
       <c r="HF6" s="1"/>
     </row>
-    <row r="7" spans="1:214" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:214">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1328,22 +1340,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:214" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:214">
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:214" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:214">
       <c r="B9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:214" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:214">
       <c r="B10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="4:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:4" ht="18.75">
       <c r="D17" s="2"/>
     </row>
   </sheetData>
@@ -1357,209 +1369,209 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:HF21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:HF22"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="108" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="36" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="36" width="3.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:214" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:214" ht="15.95" customHeight="1">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="M1" s="10" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="M1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
-      <c r="AH1" s="10"/>
-      <c r="AI1" s="10"/>
-      <c r="AJ1" s="10"/>
-      <c r="AK1" s="10"/>
-      <c r="AL1" s="10"/>
-      <c r="AM1" s="10"/>
-      <c r="AN1" s="10"/>
-      <c r="AO1" s="10"/>
-      <c r="AP1" s="10"/>
-      <c r="AQ1" s="10"/>
-      <c r="AR1" s="10"/>
-      <c r="AS1" s="10"/>
-      <c r="AT1" s="10"/>
-      <c r="AU1" s="10"/>
-    </row>
-    <row r="2" spans="1:214" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="10"/>
-      <c r="AB2" s="10"/>
-      <c r="AC2" s="10"/>
-      <c r="AD2" s="10"/>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="10"/>
-      <c r="AG2" s="10"/>
-      <c r="AH2" s="10"/>
-      <c r="AI2" s="10"/>
-      <c r="AJ2" s="10"/>
-      <c r="AK2" s="10"/>
-      <c r="AL2" s="10"/>
-      <c r="AM2" s="10"/>
-      <c r="AN2" s="10"/>
-      <c r="AO2" s="10"/>
-      <c r="AP2" s="10"/>
-      <c r="AQ2" s="10"/>
-      <c r="AR2" s="10"/>
-      <c r="AS2" s="10"/>
-      <c r="AT2" s="10"/>
-      <c r="AU2" s="10"/>
-    </row>
-    <row r="3" spans="1:214" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="10"/>
-      <c r="AB3" s="10"/>
-      <c r="AC3" s="10"/>
-      <c r="AD3" s="10"/>
-      <c r="AE3" s="10"/>
-      <c r="AF3" s="10"/>
-      <c r="AG3" s="10"/>
-      <c r="AH3" s="10"/>
-      <c r="AI3" s="10"/>
-      <c r="AJ3" s="10"/>
-      <c r="AK3" s="10"/>
-      <c r="AL3" s="10"/>
-      <c r="AM3" s="10"/>
-      <c r="AN3" s="10"/>
-      <c r="AO3" s="10"/>
-      <c r="AP3" s="10"/>
-      <c r="AQ3" s="10"/>
-      <c r="AR3" s="10"/>
-      <c r="AS3" s="10"/>
-      <c r="AT3" s="10"/>
-      <c r="AU3" s="10"/>
-    </row>
-    <row r="4" spans="1:214" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-      <c r="Z4" s="10"/>
-      <c r="AA4" s="10"/>
-      <c r="AB4" s="10"/>
-      <c r="AC4" s="10"/>
-      <c r="AD4" s="10"/>
-      <c r="AE4" s="10"/>
-      <c r="AF4" s="10"/>
-      <c r="AG4" s="10"/>
-      <c r="AH4" s="10"/>
-      <c r="AI4" s="10"/>
-      <c r="AJ4" s="10"/>
-      <c r="AK4" s="10"/>
-      <c r="AL4" s="10"/>
-      <c r="AM4" s="10"/>
-      <c r="AN4" s="10"/>
-      <c r="AO4" s="10"/>
-      <c r="AP4" s="10"/>
-      <c r="AQ4" s="10"/>
-      <c r="AR4" s="10"/>
-      <c r="AS4" s="10"/>
-      <c r="AT4" s="10"/>
-      <c r="AU4" s="10"/>
-    </row>
-    <row r="5" spans="1:214" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="14"/>
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="14"/>
+      <c r="AI1" s="14"/>
+      <c r="AJ1" s="14"/>
+      <c r="AK1" s="14"/>
+      <c r="AL1" s="14"/>
+      <c r="AM1" s="14"/>
+      <c r="AN1" s="14"/>
+      <c r="AO1" s="14"/>
+      <c r="AP1" s="14"/>
+      <c r="AQ1" s="14"/>
+      <c r="AR1" s="14"/>
+      <c r="AS1" s="14"/>
+      <c r="AT1" s="14"/>
+      <c r="AU1" s="14"/>
+    </row>
+    <row r="2" spans="1:214" ht="15.95" customHeight="1">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="14"/>
+      <c r="AE2" s="14"/>
+      <c r="AF2" s="14"/>
+      <c r="AG2" s="14"/>
+      <c r="AH2" s="14"/>
+      <c r="AI2" s="14"/>
+      <c r="AJ2" s="14"/>
+      <c r="AK2" s="14"/>
+      <c r="AL2" s="14"/>
+      <c r="AM2" s="14"/>
+      <c r="AN2" s="14"/>
+      <c r="AO2" s="14"/>
+      <c r="AP2" s="14"/>
+      <c r="AQ2" s="14"/>
+      <c r="AR2" s="14"/>
+      <c r="AS2" s="14"/>
+      <c r="AT2" s="14"/>
+      <c r="AU2" s="14"/>
+    </row>
+    <row r="3" spans="1:214" ht="15.95" customHeight="1">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14"/>
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="14"/>
+      <c r="AC3" s="14"/>
+      <c r="AD3" s="14"/>
+      <c r="AE3" s="14"/>
+      <c r="AF3" s="14"/>
+      <c r="AG3" s="14"/>
+      <c r="AH3" s="14"/>
+      <c r="AI3" s="14"/>
+      <c r="AJ3" s="14"/>
+      <c r="AK3" s="14"/>
+      <c r="AL3" s="14"/>
+      <c r="AM3" s="14"/>
+      <c r="AN3" s="14"/>
+      <c r="AO3" s="14"/>
+      <c r="AP3" s="14"/>
+      <c r="AQ3" s="14"/>
+      <c r="AR3" s="14"/>
+      <c r="AS3" s="14"/>
+      <c r="AT3" s="14"/>
+      <c r="AU3" s="14"/>
+    </row>
+    <row r="4" spans="1:214" ht="15.95" customHeight="1">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="14"/>
+      <c r="AB4" s="14"/>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="14"/>
+      <c r="AE4" s="14"/>
+      <c r="AF4" s="14"/>
+      <c r="AG4" s="14"/>
+      <c r="AH4" s="14"/>
+      <c r="AI4" s="14"/>
+      <c r="AJ4" s="14"/>
+      <c r="AK4" s="14"/>
+      <c r="AL4" s="14"/>
+      <c r="AM4" s="14"/>
+      <c r="AN4" s="14"/>
+      <c r="AO4" s="14"/>
+      <c r="AP4" s="14"/>
+      <c r="AQ4" s="14"/>
+      <c r="AR4" s="14"/>
+      <c r="AS4" s="14"/>
+      <c r="AT4" s="14"/>
+      <c r="AU4" s="14"/>
+    </row>
+    <row r="5" spans="1:214" ht="15.95" customHeight="1">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1605,108 +1617,108 @@
       <c r="AT5" s="5"/>
       <c r="AU5" s="5"/>
     </row>
-    <row r="6" spans="1:214" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="11" t="s">
+    <row r="6" spans="1:214" ht="18" customHeight="1">
+      <c r="C6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="11" t="s">
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="11" t="s">
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="11" t="s">
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="11" t="s">
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="U6" s="12"/>
-      <c r="V6" s="12"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="11" t="s">
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="Y6" s="12"/>
-      <c r="Z6" s="12"/>
-      <c r="AA6" s="12"/>
-      <c r="AB6" s="13"/>
-      <c r="AC6" s="11" t="s">
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="17"/>
+      <c r="AC6" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="AD6" s="12"/>
-      <c r="AE6" s="12"/>
-      <c r="AF6" s="13"/>
-      <c r="AG6" s="11" t="s">
+      <c r="AD6" s="16"/>
+      <c r="AE6" s="16"/>
+      <c r="AF6" s="17"/>
+      <c r="AG6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="AH6" s="12"/>
-      <c r="AI6" s="12"/>
-      <c r="AJ6" s="13"/>
-    </row>
-    <row r="7" spans="1:214" s="7" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="14">
+      <c r="AH6" s="16"/>
+      <c r="AI6" s="16"/>
+      <c r="AJ6" s="17"/>
+    </row>
+    <row r="7" spans="1:214" s="7" customFormat="1" ht="63" customHeight="1">
+      <c r="C7" s="9">
         <v>42284</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="10">
         <v>42291</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="10">
         <v>42298</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="11">
         <v>42305</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="9">
         <v>42312</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="10">
         <v>42319</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="10">
         <v>42326</v>
       </c>
-      <c r="J7" s="16">
+      <c r="J7" s="11">
         <v>42333</v>
       </c>
-      <c r="K7" s="14">
+      <c r="K7" s="9">
         <v>42340</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7" s="10">
         <v>42347</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M7" s="10">
         <v>42354</v>
       </c>
-      <c r="N7" s="15">
+      <c r="N7" s="10">
         <v>42361</v>
       </c>
-      <c r="O7" s="16">
+      <c r="O7" s="11">
         <v>42368</v>
       </c>
-      <c r="P7" s="14">
+      <c r="P7" s="9">
         <v>42375</v>
       </c>
-      <c r="Q7" s="15">
+      <c r="Q7" s="10">
         <v>42382</v>
       </c>
-      <c r="R7" s="15">
+      <c r="R7" s="10">
         <v>42389</v>
       </c>
-      <c r="S7" s="16">
+      <c r="S7" s="11">
         <v>42396</v>
       </c>
       <c r="T7" s="8">
@@ -1939,14 +1951,14 @@
       <c r="HE7" s="8"/>
       <c r="HF7" s="8"/>
     </row>
-    <row r="8" spans="1:214" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:214">
       <c r="A8" t="s">
         <v>1</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="12"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -1971,12 +1983,12 @@
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
     </row>
-    <row r="9" spans="1:214" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:214">
       <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
@@ -2000,14 +2012,14 @@
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
     </row>
-    <row r="10" spans="1:214" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:214">
       <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2029,13 +2041,13 @@
       <c r="Y10" s="6"/>
       <c r="Z10" s="6"/>
     </row>
-    <row r="11" spans="1:214" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:214">
       <c r="B11" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="E11" s="12"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -2058,9 +2070,9 @@
       <c r="Y11" s="6"/>
       <c r="Z11" s="6"/>
     </row>
-    <row r="12" spans="1:214" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:214">
       <c r="B12" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -2087,9 +2099,9 @@
       <c r="Y12" s="6"/>
       <c r="Z12" s="6"/>
     </row>
-    <row r="13" spans="1:214" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:214">
       <c r="B13" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -2116,11 +2128,14 @@
       <c r="Y13" s="6"/>
       <c r="Z13" s="6"/>
     </row>
-    <row r="14" spans="1:214" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:214">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="F14" s="12"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
@@ -2142,7 +2157,7 @@
       <c r="Y14" s="6"/>
       <c r="Z14" s="6"/>
     </row>
-    <row r="15" spans="1:214" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:214">
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -2168,8 +2183,34 @@
       <c r="Y15" s="6"/>
       <c r="Z15" s="6"/>
     </row>
-    <row r="21" spans="4:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="D21" s="2"/>
+    <row r="16" spans="1:214">
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
+    </row>
+    <row r="22" spans="4:4" ht="18.75">
+      <c r="D22" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>